<commit_message>
Aggiornato il file SENTIERI.py
</commit_message>
<xml_diff>
--- a/inputapp.xlsx
+++ b/inputapp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B87AD7-317E-41EE-B762-DCB7633CABB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF742609-58D2-4505-B1A2-441AD8CB9DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AD8CF0C8-CA00-40A0-890D-858F84AD006C}"/>
   </bookViews>
@@ -184,10 +184,10 @@
     <t xml:space="preserve">eremo del monte Barro - museo archeologico - museo etnografico </t>
   </si>
   <si>
-    <t>https://drive.google.com/uc?export=download&amp;id=1OTduecCU2ZD155QU8GYri7BTAaRuODGY</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/uc?export=download&amp;id=16_4ULTFFd2KKI-YOcXn0K_ujtIMKk5DM</t>
+    <t>https://drive.google.com/uc?id=1OTduecCU2ZD155QU8GYri7BTAaRuODGY</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?id=16_4ULTFFd2KKI-YOcXn0K_ujtIMKk5DM</t>
   </si>
 </sst>
 </file>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3F9B34-745C-41A5-B557-6D052BE4DBE6}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="L7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>